<commit_message>
add randm_forest.py and minor refactoring
</commit_message>
<xml_diff>
--- a/data/datasource.xlsx
+++ b/data/datasource.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\distanislaoj\dev\python\II40\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8298B833-0B18-4BB2-A258-F9CD8E630E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC6A9FE-E0F9-4447-9D39-A2842F2D0FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3E8DF86B-C812-4471-83AA-8677244E39DC}"/>
   </bookViews>
@@ -3821,16 +3821,16 @@
     <tableColumn id="10" xr3:uid="{E15C5808-72C4-4827-B8C4-64A3A7B75902}" uniqueName="10" name="Salary" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{4C0AA1BC-32DF-41BB-92E6-6CDDBDBA5033}" uniqueName="11" name="Termd" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{CD15032B-CE95-43EF-B6C1-0F08F2410F69}" uniqueName="12" name="PositionID" queryTableFieldId="12"/>
-    <tableColumn id="16" xr3:uid="{B716C2D7-16CA-477C-BC13-52D9B3E71D44}" uniqueName="16" name="DOB" queryTableFieldId="16" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{12C657E4-C7EE-4E83-BA37-51454AB5E00B}" uniqueName="17" name="Sex" queryTableFieldId="17" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{2963D373-8045-44BC-A372-04FEA8D4F36D}" uniqueName="22" name="DateofHire" queryTableFieldId="22" dataDxfId="5"/>
-    <tableColumn id="23" xr3:uid="{E9B596CA-6616-4624-80D1-970DB9C961C3}" uniqueName="23" name="DateofTermination" queryTableFieldId="23" dataDxfId="4"/>
-    <tableColumn id="24" xr3:uid="{87C45272-F091-4B0F-8C64-F2DF4BED79BE}" uniqueName="24" name="TermReason" queryTableFieldId="24" dataDxfId="3"/>
-    <tableColumn id="25" xr3:uid="{317D7BF9-7885-424F-BB58-6DC485F8709B}" uniqueName="25" name="EmploymentStatus" queryTableFieldId="25" dataDxfId="2"/>
-    <tableColumn id="30" xr3:uid="{40ACD9BA-808B-4DB2-AEA5-A9907F412DEB}" uniqueName="30" name="PerformanceScore" queryTableFieldId="30" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{B716C2D7-16CA-477C-BC13-52D9B3E71D44}" uniqueName="16" name="DOB" queryTableFieldId="16" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{12C657E4-C7EE-4E83-BA37-51454AB5E00B}" uniqueName="17" name="Sex" queryTableFieldId="17" dataDxfId="0"/>
+    <tableColumn id="22" xr3:uid="{2963D373-8045-44BC-A372-04FEA8D4F36D}" uniqueName="22" name="DateofHire" queryTableFieldId="22" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{E9B596CA-6616-4624-80D1-970DB9C961C3}" uniqueName="23" name="DateofTermination" queryTableFieldId="23" dataDxfId="6"/>
+    <tableColumn id="24" xr3:uid="{87C45272-F091-4B0F-8C64-F2DF4BED79BE}" uniqueName="24" name="TermReason" queryTableFieldId="24" dataDxfId="5"/>
+    <tableColumn id="25" xr3:uid="{317D7BF9-7885-424F-BB58-6DC485F8709B}" uniqueName="25" name="EmploymentStatus" queryTableFieldId="25" dataDxfId="4"/>
+    <tableColumn id="30" xr3:uid="{40ACD9BA-808B-4DB2-AEA5-A9907F412DEB}" uniqueName="30" name="PerformanceScore" queryTableFieldId="30" dataDxfId="3"/>
     <tableColumn id="32" xr3:uid="{747E30F2-DD8C-44D2-8EDF-9B5350C51F40}" uniqueName="32" name="EmpSatisfaction" queryTableFieldId="32"/>
     <tableColumn id="33" xr3:uid="{072768D0-C552-49BC-8594-C104EF507781}" uniqueName="33" name="SpecialProjectsCount" queryTableFieldId="33"/>
-    <tableColumn id="34" xr3:uid="{29DBCF9D-0F77-43DB-A36A-FBD138FAF694}" uniqueName="34" name="LastPerformanceReview_Date" queryTableFieldId="34" dataDxfId="0"/>
+    <tableColumn id="34" xr3:uid="{29DBCF9D-0F77-43DB-A36A-FBD138FAF694}" uniqueName="34" name="LastPerformanceReview_Date" queryTableFieldId="34" dataDxfId="2"/>
     <tableColumn id="35" xr3:uid="{8B443C69-54A5-42C0-AC96-29EC833210E6}" uniqueName="35" name="DaysLateLast30" queryTableFieldId="35"/>
     <tableColumn id="36" xr3:uid="{EE228CC1-34A2-4E57-91EB-B1F957C72317}" uniqueName="36" name="Absences" queryTableFieldId="36"/>
   </tableColumns>
@@ -38506,7 +38506,7 @@
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
     <col min="13" max="13" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>

</xml_diff>